<commit_message>
finalized mapping docs #27
</commit_message>
<xml_diff>
--- a/docs/CAFE to target and 1.5 - final May 21 2025.xlsx
+++ b/docs/CAFE to target and 1.5 - final May 21 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fostel\Desktop\my projects\deep cafe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaymc/Documents/workspace-accel/accelerator-core/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D1AA0C8-B94A-4129-AE5E-1563969DE9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118478C6-59A3-3D4E-9623-FF29281B3C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{9738E30D-13F0-4423-88D5-FBFA52232D50}"/>
+    <workbookView xWindow="25720" yWindow="0" windowWidth="25480" windowHeight="28800" activeTab="1" xr2:uid="{9738E30D-13F0-4423-88D5-FBFA52232D50}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="385">
   <si>
     <t>target section</t>
   </si>
@@ -1189,13 +1189,19 @@
   </si>
   <si>
     <t>target index for reference</t>
+  </si>
+  <si>
+    <t>submitter is not the same as author, submitter is who pulled the doc into accelerator</t>
+  </si>
+  <si>
+    <t>The domain doesn't include the constrained values dataverse accepts as subject, how do we map?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1215,6 +1221,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1291,7 +1309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1307,6 +1325,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1834,13 +1854,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8BE124-334E-48F9-ADED-49CDF66A81E6}">
   <dimension ref="A1:N156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O1048576"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N103" sqref="N103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="14" max="14" width="50.1640625" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>381</v>
       </c>
@@ -1866,7 +1898,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1874,7 +1906,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1882,7 +1914,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1890,7 +1922,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1898,7 +1930,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1916,7 +1948,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1924,7 +1956,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1950,7 +1982,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1968,7 +2000,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1976,7 +2008,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1984,7 +2016,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1992,7 +2024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2015,7 +2047,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2041,7 +2073,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -2064,7 +2096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2090,7 +2122,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -2098,7 +2130,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -2106,7 +2138,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -2129,7 +2161,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -2155,7 +2187,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2195,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2171,7 +2203,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -2179,7 +2211,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -2187,7 +2219,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2195,7 +2227,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2203,7 +2235,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2211,7 +2243,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -2219,7 +2251,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -2227,7 +2259,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -2235,7 +2267,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2243,7 +2275,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -2251,7 +2283,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -2274,7 +2306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2282,7 +2314,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2290,7 +2322,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2298,7 +2330,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -2306,7 +2338,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2314,7 +2346,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -2322,7 +2354,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2330,7 +2362,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2338,7 +2370,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2346,7 +2378,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2354,7 +2386,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2362,7 +2394,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -2384,8 +2416,11 @@
       <c r="L45" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N45" s="15" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -2406,7 +2441,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -2414,7 +2449,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -2422,7 +2457,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -2430,7 +2465,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -2438,7 +2473,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2456,7 +2491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2477,7 +2512,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -2485,7 +2520,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -2493,7 +2528,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -2501,7 +2536,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -2509,7 +2544,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -2517,7 +2552,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>84</v>
       </c>
@@ -2525,7 +2560,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -2533,7 +2568,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -2541,7 +2576,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -2549,7 +2584,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -2557,7 +2592,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -2565,7 +2600,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -2573,7 +2608,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>91</v>
       </c>
@@ -2581,7 +2616,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>92</v>
       </c>
@@ -2604,7 +2639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>93</v>
       </c>
@@ -2625,7 +2660,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -2633,7 +2668,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -2641,7 +2676,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -2649,7 +2684,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -2657,7 +2692,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>96</v>
       </c>
@@ -2675,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -2696,7 +2731,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>105</v>
       </c>
@@ -2704,7 +2739,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>106</v>
       </c>
@@ -2712,7 +2747,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -2720,7 +2755,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -2728,7 +2763,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -2751,7 +2786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>97</v>
       </c>
@@ -2772,7 +2807,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>98</v>
       </c>
@@ -2780,7 +2815,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>99</v>
       </c>
@@ -2788,7 +2823,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2796,7 +2831,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -2804,7 +2839,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>108</v>
       </c>
@@ -2812,7 +2847,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2820,7 +2855,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2828,7 +2863,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2836,7 +2871,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2844,7 +2879,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>109</v>
       </c>
@@ -2852,7 +2887,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>110</v>
       </c>
@@ -2860,7 +2895,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2868,7 +2903,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2876,7 +2911,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>111</v>
       </c>
@@ -2899,7 +2934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -2907,7 +2942,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2915,7 +2950,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -2923,7 +2958,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>82</v>
       </c>
@@ -2931,7 +2966,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>77</v>
       </c>
@@ -2939,7 +2974,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -2947,7 +2982,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -2955,7 +2990,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>113</v>
       </c>
@@ -2963,7 +2998,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>86</v>
       </c>
@@ -2971,7 +3006,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -2993,8 +3028,11 @@
       <c r="L103" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N103" s="16" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>115</v>
       </c>
@@ -3020,7 +3058,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -3028,7 +3066,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>82</v>
       </c>
@@ -3036,7 +3074,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>77</v>
       </c>
@@ -3044,7 +3082,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>116</v>
       </c>
@@ -3052,7 +3090,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>79</v>
       </c>
@@ -3060,7 +3098,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>80</v>
       </c>
@@ -3068,7 +3106,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -3091,7 +3129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>82</v>
       </c>
@@ -3112,7 +3150,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -3120,7 +3158,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -3128,7 +3166,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>79</v>
       </c>
@@ -3136,7 +3174,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>80</v>
       </c>
@@ -3144,7 +3182,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>119</v>
       </c>
@@ -3163,7 +3201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -3171,7 +3209,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>121</v>
       </c>
@@ -3179,7 +3217,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>122</v>
       </c>
@@ -3187,7 +3225,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>70</v>
       </c>
@@ -3195,7 +3233,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>123</v>
       </c>
@@ -3203,7 +3241,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -3211,7 +3249,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>125</v>
       </c>
@@ -3219,7 +3257,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>126</v>
       </c>
@@ -3227,7 +3265,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>127</v>
       </c>
@@ -3235,7 +3273,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>128</v>
       </c>
@@ -3243,7 +3281,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>129</v>
       </c>
@@ -3251,7 +3289,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>130</v>
       </c>
@@ -3259,7 +3297,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>131</v>
       </c>
@@ -3267,7 +3305,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>132</v>
       </c>
@@ -3275,7 +3313,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>133</v>
       </c>
@@ -3283,7 +3321,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>134</v>
       </c>
@@ -3291,7 +3329,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>135</v>
       </c>
@@ -3299,7 +3337,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>136</v>
       </c>
@@ -3307,7 +3345,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>137</v>
       </c>
@@ -3315,7 +3353,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>138</v>
       </c>
@@ -3323,7 +3361,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>139</v>
       </c>
@@ -3331,7 +3369,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>140</v>
       </c>
@@ -3339,7 +3377,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>141</v>
       </c>
@@ -3347,7 +3385,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>142</v>
       </c>
@@ -3355,7 +3393,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>143</v>
       </c>
@@ -3363,7 +3401,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>144</v>
       </c>
@@ -3371,7 +3409,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>145</v>
       </c>
@@ -3379,7 +3417,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -3387,7 +3425,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>147</v>
       </c>
@@ -3395,7 +3433,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>82</v>
       </c>
@@ -3403,7 +3441,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>148</v>
       </c>
@@ -3411,7 +3449,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -3419,7 +3457,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>150</v>
       </c>
@@ -3427,7 +3465,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>151</v>
       </c>
@@ -3435,7 +3473,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -3443,7 +3481,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>122</v>
       </c>
@@ -3451,7 +3489,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -3459,7 +3497,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -3467,7 +3505,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -3477,60 +3515,61 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L6">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L9">
-    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13:L16">
-    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19:L20">
-    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33">
-    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L67">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L72">
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L73">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L78 L45 L47">
-    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L93">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L103">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L104">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L112">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L117">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3538,18 +3577,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C97E9-A271-4C95-A6F9-0330551AB7E0}">
   <dimension ref="A1:I230"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:Q1048576"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="1.83203125" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>382</v>
       </c>
@@ -3571,14 +3610,14 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3597,7 +3636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3616,7 +3655,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3630,7 +3669,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3644,7 +3683,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3654,7 +3693,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3667,7 +3706,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3686,7 +3725,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3705,7 +3744,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3724,7 +3763,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3738,7 +3777,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3757,7 +3796,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3765,7 +3804,7 @@
       <c r="C14" s="2"/>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3784,7 +3823,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3803,7 +3842,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3822,7 +3861,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3841,7 +3880,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3855,7 +3894,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3874,7 +3913,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3888,7 +3927,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3907,7 +3946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3926,7 +3965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3940,7 +3979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3954,7 +3993,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3968,7 +4007,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3987,7 +4026,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4001,7 +4040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -4015,7 +4054,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -4029,7 +4068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -4043,7 +4082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4057,7 +4096,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4071,7 +4110,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4085,7 +4124,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4099,7 +4138,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4113,7 +4152,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4121,7 +4160,7 @@
       <c r="C37" s="2"/>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4140,7 +4179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -4159,7 +4198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -4178,14 +4217,14 @@
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="10"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="10"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -4204,7 +4243,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4220,7 +4259,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4234,7 +4273,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4248,7 +4287,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4262,7 +4301,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4276,7 +4315,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4290,7 +4329,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4304,7 +4343,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -4323,7 +4362,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -4332,7 +4371,7 @@
       <c r="D51" s="2"/>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -4346,7 +4385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4365,7 +4404,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4379,7 +4418,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4393,7 +4432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4407,7 +4446,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4426,7 +4465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4445,7 +4484,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4464,7 +4503,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -4483,7 +4522,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -4502,7 +4541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -4517,7 +4556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4536,7 +4575,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>61.5</v>
       </c>
@@ -4549,7 +4588,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>62</v>
       </c>
@@ -4568,7 +4607,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>62.5</v>
       </c>
@@ -4581,7 +4620,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>63</v>
       </c>
@@ -4600,7 +4639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>64</v>
       </c>
@@ -4619,7 +4658,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>65</v>
       </c>
@@ -4638,7 +4677,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>66</v>
       </c>
@@ -4657,7 +4696,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>67</v>
       </c>
@@ -4676,7 +4715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>68</v>
       </c>
@@ -4695,14 +4734,14 @@
         <v>220</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="10"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="10"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>69</v>
       </c>
@@ -4721,7 +4760,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>70</v>
       </c>
@@ -4740,7 +4779,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>71</v>
       </c>
@@ -4759,7 +4798,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>72</v>
       </c>
@@ -4778,7 +4817,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>73</v>
       </c>
@@ -4797,7 +4836,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>74</v>
       </c>
@@ -4808,7 +4847,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>75</v>
       </c>
@@ -4822,7 +4861,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>76</v>
       </c>
@@ -4836,7 +4875,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>77</v>
       </c>
@@ -4855,7 +4894,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>78</v>
       </c>
@@ -4874,7 +4913,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>79</v>
       </c>
@@ -4889,7 +4928,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>80</v>
       </c>
@@ -4904,7 +4943,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>81</v>
       </c>
@@ -4919,7 +4958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>82</v>
       </c>
@@ -4933,7 +4972,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>83</v>
       </c>
@@ -4947,7 +4986,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>84</v>
       </c>
@@ -4961,7 +5000,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>85</v>
       </c>
@@ -4969,7 +5008,7 @@
       <c r="C90" s="2"/>
       <c r="E90" s="10"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>86</v>
       </c>
@@ -4988,7 +5027,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>87</v>
       </c>
@@ -5007,7 +5046,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>88</v>
       </c>
@@ -5026,7 +5065,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>89</v>
       </c>
@@ -5045,7 +5084,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>90</v>
       </c>
@@ -5054,7 +5093,7 @@
       <c r="D95" s="2"/>
       <c r="E95" s="10"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>91</v>
       </c>
@@ -5074,7 +5113,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>92</v>
       </c>
@@ -5093,7 +5132,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>93</v>
       </c>
@@ -5112,7 +5151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>94</v>
       </c>
@@ -5131,7 +5170,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>95</v>
       </c>
@@ -5150,7 +5189,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>96</v>
       </c>
@@ -5164,7 +5203,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>97</v>
       </c>
@@ -5178,7 +5217,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>98</v>
       </c>
@@ -5192,7 +5231,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>99</v>
       </c>
@@ -5206,7 +5245,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>100</v>
       </c>
@@ -5220,7 +5259,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>101</v>
       </c>
@@ -5239,7 +5278,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>102</v>
       </c>
@@ -5258,7 +5297,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>103</v>
       </c>
@@ -5277,7 +5316,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>104</v>
       </c>
@@ -5296,7 +5335,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>105</v>
       </c>
@@ -5315,7 +5354,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>106</v>
       </c>
@@ -5334,7 +5373,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>107</v>
       </c>
@@ -5348,7 +5387,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>108</v>
       </c>
@@ -5362,7 +5401,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>109</v>
       </c>
@@ -5376,7 +5415,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>110</v>
       </c>
@@ -5390,7 +5429,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>111</v>
       </c>
@@ -5404,7 +5443,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>112</v>
       </c>
@@ -5412,7 +5451,7 @@
       <c r="C117" s="2"/>
       <c r="E117" s="10"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>113</v>
       </c>
@@ -5431,7 +5470,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>114</v>
       </c>
@@ -5450,7 +5489,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>115</v>
       </c>
@@ -5469,7 +5508,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>116</v>
       </c>
@@ -5488,7 +5527,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>117</v>
       </c>
@@ -5507,7 +5546,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>118</v>
       </c>
@@ -5526,7 +5565,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>119</v>
       </c>
@@ -5545,7 +5584,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>120</v>
       </c>
@@ -5564,7 +5603,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>121</v>
       </c>
@@ -5583,7 +5622,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>122</v>
       </c>
@@ -5592,7 +5631,7 @@
       <c r="D127" s="2"/>
       <c r="E127" s="10"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>123</v>
       </c>
@@ -5617,7 +5656,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>124</v>
       </c>
@@ -5636,7 +5675,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>125</v>
       </c>
@@ -5655,7 +5694,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>126</v>
       </c>
@@ -5674,7 +5713,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>127</v>
       </c>
@@ -5693,7 +5732,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>128</v>
       </c>
@@ -5701,7 +5740,7 @@
       <c r="C133" s="2"/>
       <c r="E133" s="10"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>129</v>
       </c>
@@ -5723,7 +5762,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>130</v>
       </c>
@@ -5739,7 +5778,7 @@
       </c>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>131</v>
       </c>
@@ -5757,7 +5796,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>132</v>
       </c>
@@ -5776,7 +5815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>133</v>
       </c>
@@ -5795,7 +5834,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>134</v>
       </c>
@@ -5814,7 +5853,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>135</v>
       </c>
@@ -5833,7 +5872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>136</v>
       </c>
@@ -5852,7 +5891,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>137</v>
       </c>
@@ -5871,7 +5910,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>138</v>
       </c>
@@ -5890,7 +5929,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>139</v>
       </c>
@@ -5904,7 +5943,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>140</v>
       </c>
@@ -5918,7 +5957,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>141</v>
       </c>
@@ -5932,7 +5971,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>142</v>
       </c>
@@ -5946,7 +5985,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>143</v>
       </c>
@@ -5971,7 +6010,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>144</v>
       </c>
@@ -5986,7 +6025,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>145</v>
       </c>
@@ -6005,7 +6044,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>146</v>
       </c>
@@ -6024,7 +6063,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>147</v>
       </c>
@@ -6043,7 +6082,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>148</v>
       </c>
@@ -6062,7 +6101,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>149</v>
       </c>
@@ -6081,7 +6120,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>150</v>
       </c>
@@ -6100,7 +6139,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>151</v>
       </c>
@@ -6119,7 +6158,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>152</v>
       </c>
@@ -6133,7 +6172,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>153</v>
       </c>
@@ -6147,7 +6186,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>154</v>
       </c>
@@ -6161,7 +6200,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>155</v>
       </c>
@@ -6181,7 +6220,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>156</v>
       </c>
@@ -6195,7 +6234,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>157</v>
       </c>
@@ -6203,7 +6242,7 @@
       <c r="C162" s="2"/>
       <c r="E162" s="10"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>158</v>
       </c>
@@ -6217,7 +6256,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>159</v>
       </c>
@@ -6231,7 +6270,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>160</v>
       </c>
@@ -6245,7 +6284,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>161</v>
       </c>
@@ -6259,7 +6298,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>162</v>
       </c>
@@ -6273,7 +6312,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>163</v>
       </c>
@@ -6287,7 +6326,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>164</v>
       </c>
@@ -6301,7 +6340,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>165</v>
       </c>
@@ -6315,7 +6354,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>166</v>
       </c>
@@ -6329,7 +6368,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>167</v>
       </c>
@@ -6343,7 +6382,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>168</v>
       </c>
@@ -6357,7 +6396,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>169</v>
       </c>
@@ -6371,7 +6410,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>170</v>
       </c>
@@ -6385,7 +6424,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>171</v>
       </c>
@@ -6393,7 +6432,7 @@
       <c r="C176" s="2"/>
       <c r="E176" s="10"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>172</v>
       </c>
@@ -6412,7 +6451,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>173</v>
       </c>
@@ -6431,7 +6470,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>174</v>
       </c>
@@ -6450,7 +6489,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>175</v>
       </c>
@@ -6464,7 +6503,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>176</v>
       </c>
@@ -6478,7 +6517,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>177</v>
       </c>
@@ -6492,7 +6531,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>178</v>
       </c>
@@ -6506,7 +6545,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>179</v>
       </c>
@@ -6520,7 +6559,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>180</v>
       </c>
@@ -6534,7 +6573,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>181</v>
       </c>
@@ -6553,7 +6592,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>182</v>
       </c>
@@ -6567,7 +6606,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>183</v>
       </c>
@@ -6575,7 +6614,7 @@
       <c r="C188" s="2"/>
       <c r="E188" s="10"/>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>184</v>
       </c>
@@ -6589,7 +6628,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>185</v>
       </c>
@@ -6603,7 +6642,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>186</v>
       </c>
@@ -6617,7 +6656,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>187</v>
       </c>
@@ -6631,7 +6670,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>188</v>
       </c>
@@ -6639,7 +6678,7 @@
       <c r="C193" s="2"/>
       <c r="E193" s="10"/>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>189</v>
       </c>
@@ -6653,7 +6692,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>190</v>
       </c>
@@ -6667,7 +6706,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>191</v>
       </c>
@@ -6681,7 +6720,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>192</v>
       </c>
@@ -6695,7 +6734,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>193</v>
       </c>
@@ -6709,7 +6748,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>194</v>
       </c>
@@ -6723,7 +6762,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>195</v>
       </c>
@@ -6737,7 +6776,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>196</v>
       </c>
@@ -6751,7 +6790,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>197</v>
       </c>
@@ -6765,7 +6804,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
         <v>198</v>
       </c>
@@ -6779,7 +6818,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>199</v>
       </c>
@@ -6793,7 +6832,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
         <v>200</v>
       </c>
@@ -6807,7 +6846,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>201</v>
       </c>
@@ -6826,7 +6865,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>202</v>
       </c>
@@ -6845,7 +6884,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>203</v>
       </c>
@@ -6859,7 +6898,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>204</v>
       </c>
@@ -6873,7 +6912,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>205</v>
       </c>
@@ -6887,7 +6926,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>206</v>
       </c>
@@ -6895,7 +6934,7 @@
       <c r="C211" s="2"/>
       <c r="E211" s="10"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>207</v>
       </c>
@@ -6914,7 +6953,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>208</v>
       </c>
@@ -6933,7 +6972,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>209</v>
       </c>
@@ -6947,7 +6986,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>210</v>
       </c>
@@ -6961,7 +7000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>211</v>
       </c>
@@ -6975,7 +7014,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>212</v>
       </c>
@@ -6994,7 +7033,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>213</v>
       </c>
@@ -7013,7 +7052,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>214</v>
       </c>
@@ -7032,7 +7071,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>215</v>
       </c>
@@ -7057,7 +7096,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>216</v>
       </c>
@@ -7075,7 +7114,7 @@
       <c r="H221" s="2"/>
       <c r="I221" s="2"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>217</v>
       </c>
@@ -7094,7 +7133,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>218</v>
       </c>
@@ -7110,7 +7149,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>219</v>
       </c>
@@ -7129,7 +7168,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
         <v>220</v>
       </c>
@@ -7148,7 +7187,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>221</v>
       </c>
@@ -7164,7 +7203,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>222</v>
       </c>
@@ -7180,7 +7219,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>223</v>
       </c>
@@ -7199,18 +7238,18 @@
         <v>368</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B229" s="9"/>
       <c r="E229" s="9"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B230" s="9"/>
       <c r="E230" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I568" xr:uid="{083C97E9-A271-4C95-A6F9-0330551AB7E0}"/>
   <conditionalFormatting sqref="G128 G101:G105 G133 G112:G117 G144:G176 G180:G185 G187:G205 G208:G212 G214:G220 G224 G222 G1:G99">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>